<commit_message>
Update GitHub backend integration in streamlit_app.py
</commit_message>
<xml_diff>
--- a/DAP_protocol_extended.xlsx
+++ b/DAP_protocol_extended.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10526"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10608"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/f0212e7307df41dd/Kim lab (2024-)/Programe/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/f0212e7307df41dd/Kim lab (2024-)/Programe/DDS/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="14" documentId="8_{510C3773-BBFC-DB4E-ABCC-749D2482CF2B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{12C27140-4A74-EB4B-9603-85911611FBEE}"/>
+  <xr:revisionPtr revIDLastSave="29" documentId="8_{510C3773-BBFC-DB4E-ABCC-749D2482CF2B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A76A9D02-4D13-4449-B80D-2432106AA4C1}"/>
   <bookViews>
-    <workbookView xWindow="4220" yWindow="3740" windowWidth="18440" windowHeight="15380" xr2:uid="{8BCC1942-A0A5-4944-B994-D179F7DFE306}"/>
+    <workbookView xWindow="23040" yWindow="500" windowWidth="23040" windowHeight="24360" xr2:uid="{8BCC1942-A0A5-4944-B994-D179F7DFE306}"/>
   </bookViews>
   <sheets>
     <sheet name="DAP_protocol_extended" sheetId="1" r:id="rId1"/>
@@ -941,7 +941,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -979,6 +979,9 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="16" fillId="33" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1037,6 +1040,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1358,8 +1365,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4FA255B5-DC9C-F545-A72E-26102A24A80C}">
   <dimension ref="A1:F135"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A79" zoomScale="108" workbookViewId="0">
-      <selection activeCell="D100" sqref="D100"/>
+    <sheetView tabSelected="1" topLeftCell="A54" zoomScale="108" workbookViewId="0">
+      <selection activeCell="C111" sqref="C111:C116"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="18"/>
@@ -2610,7 +2617,7 @@
         <v>54</v>
       </c>
       <c r="D73" s="2">
-        <v>93.3</v>
+        <v>98.3</v>
       </c>
       <c r="E73" s="2"/>
       <c r="F73" s="2"/>
@@ -2728,15 +2735,15 @@
       <c r="B80" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="C80" s="12" t="s">
-        <v>41</v>
-      </c>
-      <c r="D80" s="12"/>
-      <c r="E80" s="12" t="s">
-        <v>43</v>
-      </c>
-      <c r="F80" s="12" t="s">
-        <v>45</v>
+      <c r="C80" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="D80" s="2"/>
+      <c r="E80" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="F80" s="2" t="s">
+        <v>24</v>
       </c>
     </row>
     <row r="81" spans="1:6">
@@ -2746,15 +2753,15 @@
       <c r="B81" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="C81" s="2" t="s">
-        <v>63</v>
-      </c>
-      <c r="D81" s="2"/>
-      <c r="E81" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="F81" s="2" t="s">
-        <v>24</v>
+      <c r="C81" s="12" t="s">
+        <v>41</v>
+      </c>
+      <c r="D81" s="12"/>
+      <c r="E81" s="12" t="s">
+        <v>43</v>
+      </c>
+      <c r="F81" s="12" t="s">
+        <v>45</v>
       </c>
     </row>
     <row r="82" spans="1:6">
@@ -2851,11 +2858,11 @@
       <c r="B88" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="C88" s="7" t="s">
+      <c r="C88" s="13" t="s">
         <v>54</v>
       </c>
-      <c r="D88" s="2">
-        <v>93.3</v>
+      <c r="D88" s="13">
+        <v>98.3</v>
       </c>
       <c r="E88" s="2"/>
       <c r="F88" s="2"/>
@@ -2867,10 +2874,10 @@
       <c r="B89" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="C89" s="7" t="s">
+      <c r="C89" s="13" t="s">
         <v>50</v>
       </c>
-      <c r="D89" s="7">
+      <c r="D89" s="13">
         <v>1</v>
       </c>
       <c r="E89" s="2"/>
@@ -2973,15 +2980,15 @@
       <c r="B95" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="C95" s="12" t="s">
-        <v>41</v>
-      </c>
-      <c r="D95" s="12"/>
-      <c r="E95" s="12" t="s">
-        <v>43</v>
-      </c>
-      <c r="F95" s="12" t="s">
-        <v>45</v>
+      <c r="C95" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="D95" s="2"/>
+      <c r="E95" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="F95" s="2" t="s">
+        <v>24</v>
       </c>
     </row>
     <row r="96" spans="1:6">
@@ -2991,15 +2998,15 @@
       <c r="B96" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="C96" s="2" t="s">
-        <v>63</v>
-      </c>
-      <c r="D96" s="2"/>
-      <c r="E96" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="F96" s="2" t="s">
-        <v>24</v>
+      <c r="C96" s="12" t="s">
+        <v>41</v>
+      </c>
+      <c r="D96" s="12"/>
+      <c r="E96" s="12" t="s">
+        <v>43</v>
+      </c>
+      <c r="F96" s="12" t="s">
+        <v>45</v>
       </c>
     </row>
     <row r="97" spans="1:6">
@@ -3054,11 +3061,11 @@
       <c r="B100" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="C100" s="7" t="s">
+      <c r="C100" s="13" t="s">
         <v>54</v>
       </c>
-      <c r="D100" s="2">
-        <v>93.3</v>
+      <c r="D100" s="13">
+        <v>98.3</v>
       </c>
       <c r="E100" s="2"/>
       <c r="F100" s="2"/>
@@ -3070,10 +3077,10 @@
       <c r="B101" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="C101" s="7" t="s">
+      <c r="C101" s="13" t="s">
         <v>50</v>
       </c>
-      <c r="D101" s="7">
+      <c r="D101" s="13">
         <v>1</v>
       </c>
       <c r="E101" s="2"/>
@@ -3194,7 +3201,7 @@
       <c r="B108" s="1" t="s">
         <v>81</v>
       </c>
-      <c r="C108" s="1" t="s">
+      <c r="C108" s="8" t="s">
         <v>22</v>
       </c>
       <c r="E108" s="1" t="s">
@@ -3211,10 +3218,10 @@
       <c r="B109" s="2" t="s">
         <v>79</v>
       </c>
-      <c r="C109" s="7" t="s">
+      <c r="C109" s="13" t="s">
         <v>54</v>
       </c>
-      <c r="D109" s="2">
+      <c r="D109" s="13">
         <v>98.4</v>
       </c>
       <c r="E109" s="2"/>
@@ -3227,10 +3234,10 @@
       <c r="B110" s="2" t="s">
         <v>79</v>
       </c>
-      <c r="C110" s="7" t="s">
+      <c r="C110" s="13" t="s">
         <v>50</v>
       </c>
-      <c r="D110" s="7">
+      <c r="D110" s="13">
         <v>1</v>
       </c>
       <c r="E110" s="2"/>

</xml_diff>